<commit_message>
ran a ton of runs with all configs
</commit_message>
<xml_diff>
--- a/Warehouse/AB/judgement_logs_run4o.xlsx
+++ b/Warehouse/AB/judgement_logs_run4o.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,19 +456,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;31;03.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_10;45;32.json</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached for the theme for spirit week, so the function for no consensus has been called.
+MSG: None
+MSG: The selected theme for spirit week is Crazy Hat Day!
 </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_consensus, </t>
+          <t xml:space="preserve">they_came_to_a_compromise, , crazy_hat_day_was_selected, </t>
         </is>
       </c>
     </row>
@@ -478,13 +479,13 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;42;30.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_10;57;02.json</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Since there was no consensus reached on the theme for spirit week, I have called the function indicating no consensus.
+MSG: There was no consensus reached regarding the theme for spirit week.
 </t>
         </is>
       </c>
@@ -500,13 +501,13 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;41;13.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_11;02;18.json</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached regarding the theme for spirit week.
+MSG: There was no consensus reached on the theme for spirit week.
 </t>
         </is>
       </c>
@@ -522,13 +523,13 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;37;16.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_10;51;16.json</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached regarding the theme for spirit week.
+MSG: There was no consensus on the theme for spirit week.
 </t>
         </is>
       </c>
@@ -544,19 +545,19 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;34;28.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_10;53;09.json</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The theme selected for spirit week is Crazy Sock Day.
+MSG: The outcome of the discussion resulted in no consensus on the theme for spirit week.
 </t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve">crazy_sock_day_was_selected, </t>
+          <t xml:space="preserve">no_consensus, </t>
         </is>
       </c>
     </row>
@@ -566,19 +567,19 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;35;02.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_10;58;00.json</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The theme selected for spirit week is Crazy Sock Day, as both Amy and John came to a compromise on this idea.
+MSG: It seems there was no consensus reached regarding the theme for spirit week.
 </t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">they_came_to_a_compromise, </t>
+          <t xml:space="preserve">no_consensus, </t>
         </is>
       </c>
     </row>
@@ -588,13 +589,13 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;46;50.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_11;00;35.json</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached regarding the theme for spirit week.
+MSG: There was no consensus on the theme for spirit week.
 </t>
         </is>
       </c>
@@ -610,13 +611,13 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;40;25.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_10;47;55.json</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has resulted in no consensus.
+MSG: There was no consensus reached for the theme of spirit week, so the appropriate action has been taken.
 </t>
         </is>
       </c>
@@ -632,19 +633,19 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;28;28.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_11;00;06.json</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The selected theme for spirit week is "Crazy Hat and Sock Day."
+MSG: Since there was no consensus reached, I have called the function no_consensus.
 </t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve">they_came_to_a_compromise, </t>
+          <t xml:space="preserve">no_consensus, </t>
         </is>
       </c>
     </row>
@@ -654,7 +655,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;18;38.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_10;50;54.json</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -676,19 +677,19 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;48;48.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_10;52;18.json</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The theme for spirit week is Crazy Sock Day!
+MSG: It appears that there was no consensus reached regarding the theme for spirit week.
 </t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve">crazy_sock_day_was_selected, </t>
+          <t xml:space="preserve">no_consensus, </t>
         </is>
       </c>
     </row>
@@ -698,13 +699,13 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;38;22.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_10;58;55.json</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Since there was no consensus reached during the discussion, I have called the function indicating that there is no consensus.
+MSG: There was no consensus reached on the theme for spirit week.
 </t>
         </is>
       </c>
@@ -720,13 +721,13 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;32;22.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_10;56;04.json</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached for the theme of spirit week.
+MSG: There was no consensus reached on the theme for spirit week, so I have called the function indicating that.
 </t>
         </is>
       </c>
@@ -742,13 +743,13 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;35;55.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_10;46;10.json</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus on the theme for spirit week.
+MSG: There was no consensus reached regarding the theme for spirit week.
 </t>
         </is>
       </c>
@@ -764,13 +765,13 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;45;02.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_11;03;56.json</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision for the theme of spirit week resulted in no consensus.
+MSG: There was no consensus reached on the theme for spirit week.
 </t>
         </is>
       </c>
@@ -786,19 +787,19 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;30;13.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_10;49;45.json</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The theme for spirit week that was selected is Crazy Sock Day.
+MSG: There was no consensus reached between the two parties on the theme for spirit week.
 </t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t xml:space="preserve">they_came_to_a_compromise, </t>
+          <t xml:space="preserve">no_consensus, </t>
         </is>
       </c>
     </row>
@@ -808,13 +809,13 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;22;22.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_10;55;30.json</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Since there was no consensus between the parties involved, I called the function for no consensus.
+MSG: It appears there was no consensus reached regarding the theme for spirit week.
 </t>
         </is>
       </c>
@@ -830,13 +831,13 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;21;36.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_11;01;24.json</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached regarding the theme for spirit week.
+MSG: There was no consensus reached on the theme for spirit week.
 </t>
         </is>
       </c>
@@ -852,13 +853,13 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;23;14.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_10;50;14.json</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The result is that there was no consensus reached for the theme for spirit week.
+MSG: The outcome of the discussion was that there was no consensus regarding the theme for spirit week.
 </t>
         </is>
       </c>
@@ -874,13 +875,13 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;24;47.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_11;05;12.json</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week, so the decision has been made accordingly.
+MSG: Since there was no consensus reached, the function for no consensus has been called.
 </t>
         </is>
       </c>
@@ -896,13 +897,13 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;43;49.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_10;59;36.json</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Since there was no consensus reached on the theme for spirit week, I have called the function for no consensus.
+MSG: There was no consensus reached regarding the theme for spirit week.
 </t>
         </is>
       </c>
@@ -918,19 +919,19 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;47;56.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_10;54;26.json</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week, so I have called the function for no consensus.
+MSG: The outcome of the discussion is that they came to a compromise, which allows for both themes to be recognized.
 </t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_consensus, </t>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
         </is>
       </c>
     </row>
@@ -940,13 +941,13 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;46;06.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_10;45;05.json</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The result is that there was no consensus reached on the theme for spirit week.
+MSG: It appears that there was no consensus reached regarding the theme for spirit week.
 </t>
         </is>
       </c>
@@ -962,13 +963,13 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;20;33.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_10;47;06.json</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Since there was no consensus between the two options, I have called the function for no consensus.
+MSG: There was no consensus reached on the theme for spirit week.
 </t>
         </is>
       </c>
@@ -984,7 +985,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;26;30.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_11;03;08.json</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1006,13 +1007,13 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;19;40.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_10;54;52.json</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week.
+MSG: The decision reached was that there was no consensus on the theme for spirit week.
 </t>
         </is>
       </c>
@@ -1028,13 +1029,13 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;33;32.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_10;58;27.json</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision for the theme of spirit week resulted in no consensus.
+MSG: The outcome of the discussion was that there was no consensus reached.
 </t>
         </is>
       </c>
@@ -1050,61 +1051,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;27;26.json</t>
+          <t>./Warehouse/AB/run4o_discovery_03_28_2025 at_11;04;48.json</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision for spirit week is to celebrate both Crazy Hat Day and Crazy Sock Day as a compromise!
+MSG: There was no consensus on the theme for spirit week, so I have called the function for no consensus.
 </t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
-        <is>
-          <t xml:space="preserve">they_came_to_a_compromise, </t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;24;06.json</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MSG: None
-MSG: The outcome of the discussion resulted in no consensus being reached for the spirit week theme.
-</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t xml:space="preserve">no_consensus, </t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>./Warehouse/AB/run4o_discovery_03_27_2025 at_22;29;14.json</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MSG: None
-MSG: There was no consensus on the theme for spirit week.
-</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
         <is>
           <t xml:space="preserve">no_consensus, </t>
         </is>

</xml_diff>